<commit_message>
adjust qa process and cleanup
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t xml:space="preserve">Run Date</t>
   </si>
@@ -45,30 +45,72 @@
     <t xml:space="preserve">Test IDs</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.gehealthcare.com/products/ultrasound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-03,TC-04,TC-05,TC-06,TC-07,TC-09,TC-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page Pass?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP Status</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.gehealthcare.com/</t>
   </si>
   <si>
-    <t xml:space="preserve">USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-01,TC-02,TC-03,TC-04,TC-05,TC-06,TC-09,TC-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.com/products/imaging</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-03,TC-04,TC-05,TC-06,TC-07,TC-09,TC-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.com/products/bone-and-metabolic-health</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-03,TC-04,TC-05,TC-06,TC-08,TC-09,TC-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.gehealthcare.com/products/ultrasound</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.com/products/ultrasound/voluson</t>
   </si>
   <si>
@@ -81,9 +123,6 @@
     <t xml:space="preserve">https://www.gehealthcare.com/products/molecular-imaging-agents</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-03,TC-04,TC-05,TC-06,TC-10,TC-09,TC-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.com/products/molecular-imaging-agents/cerianna</t>
   </si>
   <si>
@@ -93,24 +132,15 @@
     <t xml:space="preserve">https://www.gehealthcare.com/products/contrast-media/omnipaque</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-03,TC-04,TC-05,TC-06,TC-09,TC-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.com/insights?showPopup=false</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-03,TC-04,TC-05,TC-06,TC-11,TC-09,TC-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.com/about/newsroom</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gehealthcare.co.uk/</t>
   </si>
   <si>
-    <t xml:space="preserve">UK</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.co.uk/products/imaging</t>
   </si>
   <si>
@@ -147,12 +177,6 @@
     <t xml:space="preserve">https://www.gehealthcare.de/</t>
   </si>
   <si>
-    <t xml:space="preserve">DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-01,TC-02,TC-03,TC-04,TC-05,TC-06,TC-13,TC-09,TC-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.de/products/imaging</t>
   </si>
   <si>
@@ -165,9 +189,6 @@
     <t xml:space="preserve">https://www.gehealthcare.de/products/contrast-media/omnipaque</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-03,TC-04,TC-05,TC-06,TC-12,TC-09,TC-14</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.de/products/nuclear-imaging-agents</t>
   </si>
   <si>
@@ -183,9 +204,6 @@
     <t xml:space="preserve">https://www.gehealthcare.fr/</t>
   </si>
   <si>
-    <t xml:space="preserve">FR</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.fr/products/imaging</t>
   </si>
   <si>
@@ -201,9 +219,6 @@
     <t xml:space="preserve">https://www.gehealthcare.in/</t>
   </si>
   <si>
-    <t xml:space="preserve">IN</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.gehealthcare.in/products/imaging</t>
   </si>
   <si>
@@ -232,54 +247,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.gehealthcare.in/products/diagnostic-ecg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page Pass?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTTP Status</t>
   </si>
 </sst>
 </file>
@@ -565,8 +532,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblURLs" displayName="tblURLs" ref="A1:B51" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:B51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tblURLs" displayName="tblURLs" ref="A1:B2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:B2"/>
   <tableColumns count="2">
     <tableColumn id="1" name="URL"/>
     <tableColumn id="2" name="Region"/>
@@ -753,8 +720,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="2" sqref="A16 V16 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -799,15 +766,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N47" activeCellId="0" sqref="N47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V16" activeCellId="1" sqref="A16 V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="113.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.72"/>
   </cols>
   <sheetData>
@@ -818,560 +785,70 @@
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1394,7 +871,7 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="2" sqref="A16 V16 D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1408,302 +885,302 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>